<commit_message>
commit apres test masque
</commit_message>
<xml_diff>
--- a/admin/upload/EXPORT_DATA_STAT_AUTO.xlsx
+++ b/admin/upload/EXPORT_DATA_STAT_AUTO.xlsx
@@ -15,30 +15,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Nom et prénom</t>
   </si>
   <si>
-    <t>comprehension</t>
+    <t>grammaire</t>
+  </si>
+  <si>
+    <t>expression de text</t>
+  </si>
+  <si>
+    <t>resume</t>
+  </si>
+  <si>
+    <t>fanadihadiana lahatsoratra</t>
   </si>
   <si>
     <t>famakafakan-kevitra</t>
   </si>
   <si>
-    <t>expression ecrite</t>
-  </si>
-  <si>
-    <t>literatiora</t>
-  </si>
-  <si>
-    <t>fanadihadiana lahatsoratra</t>
-  </si>
-  <si>
-    <t>vocabulaire</t>
-  </si>
-  <si>
-    <t>Sahaza</t>
+    <t>probabilite</t>
+  </si>
+  <si>
+    <t>statistique</t>
+  </si>
+  <si>
+    <t>geographie</t>
+  </si>
+  <si>
+    <t>histoire</t>
+  </si>
+  <si>
+    <t>geologie</t>
+  </si>
+  <si>
+    <t>suite numerique</t>
+  </si>
+  <si>
+    <t>fonction</t>
+  </si>
+  <si>
+    <t>interference mecanique</t>
+  </si>
+  <si>
+    <t>reproduction humaine</t>
+  </si>
+  <si>
+    <t>vibration sonore</t>
+  </si>
+  <si>
+    <t>interference lumineuse</t>
+  </si>
+  <si>
+    <t>genetique</t>
+  </si>
+  <si>
+    <t>RAMANANDRAIBE</t>
+  </si>
+  <si>
+    <t>]15,20]</t>
+  </si>
+  <si>
+    <t>[10]</t>
   </si>
 </sst>
 </file>
@@ -377,7 +416,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,7 +424,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,28 +446,88 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2" t="s">
+        <v>20</v>
       </c>
       <c r="G2">
         <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>